<commit_message>
Completed 2 paths and added timestamps on the expirment script
</commit_message>
<xml_diff>
--- a/path3_experiments.xlsx
+++ b/path3_experiments.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6396E48F-59D0-4C52-A25E-6859A395DC7B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +19,34 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>Test Point ID</t>
+  </si>
+  <si>
+    <t>Time Window (s)</t>
+  </si>
+  <si>
+    <t>Algorithm Window (s)</t>
+  </si>
+  <si>
+    <t>Mean Distance Error</t>
+  </si>
+  <si>
+    <t>txPower Calibration</t>
+  </si>
+  <si>
+    <t>Overall Mean Error</t>
+  </si>
+  <si>
+    <t>No. Estimations</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -49,8 +76,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +360,213 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" customWidth="1"/>
+    <col min="5" max="6" width="17.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="E15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E17" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added optimisation algorithm and full testing environment
</commit_message>
<xml_diff>
--- a/path3_experiments.xlsx
+++ b/path3_experiments.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6396E48F-59D0-4C52-A25E-6859A395DC7B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B4C243B-6C79-4121-8FE1-40DB4DA1507B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="111">
   <si>
     <t>Test Point ID</t>
   </si>
@@ -41,13 +41,325 @@
   </si>
   <si>
     <t>No. Estimations</t>
+  </si>
+  <si>
+    <t>Number of estimated location: 129</t>
+  </si>
+  <si>
+    <t>Number of times the interval between timestamps is bigger than 3 seconds: 505</t>
+  </si>
+  <si>
+    <t>Test Point: 0  Number of Estimated Locations: 10  Mean Distance Error: 4.5015106189922625</t>
+  </si>
+  <si>
+    <t>Test Point: 1  Number of Estimated Locations: 7  Mean Distance Error: 4.808809401173978</t>
+  </si>
+  <si>
+    <t>Test Point: 2  Number of Estimated Locations: 8  Mean Distance Error: 4.358427286722411</t>
+  </si>
+  <si>
+    <t>Test Point: 3  Number of Estimated Locations: 5  Mean Distance Error: 3.5201902507083993</t>
+  </si>
+  <si>
+    <t>Test Point: 4  Number of Estimated Locations: 6  Mean Distance Error: 2.6248427813437054</t>
+  </si>
+  <si>
+    <t>Test Point: 5  Number of Estimated Locations: 6  Mean Distance Error: 8.447451004809635</t>
+  </si>
+  <si>
+    <t>Test Point: 6  Number of Estimated Locations: 7  Mean Distance Error: 6.504713875334309</t>
+  </si>
+  <si>
+    <t>Test Point: 7  Number of Estimated Locations: 9  Mean Distance Error: 6.818609202839786</t>
+  </si>
+  <si>
+    <t>Test Point: 8  Number of Estimated Locations: 8  Mean Distance Error: 3.925201919103815</t>
+  </si>
+  <si>
+    <t>Test Point: 9  Number of Estimated Locations: 9  Mean Distance Error: 4.799027511249574</t>
+  </si>
+  <si>
+    <t>Test Point: 10  Number of Estimated Locations: 10  Mean Distance Error: 4.582431751304332</t>
+  </si>
+  <si>
+    <t>Test Point: 11  Number of Estimated Locations: 10  Mean Distance Error: 3.3254315500590166</t>
+  </si>
+  <si>
+    <t>Test Point: 12  Number of Estimated Locations: 8  Mean Distance Error: 1.777054635758733</t>
+  </si>
+  <si>
+    <t>Test Point: 13  Number of Estimated Locations: 7  Mean Distance Error: 2.7083371621219654</t>
+  </si>
+  <si>
+    <t>Test Point: 14  Number of Estimated Locations: 5  Mean Distance Error: 10.45132704787036</t>
+  </si>
+  <si>
+    <t>Overall Mean Distance Error: 4.876891066626152</t>
+  </si>
+  <si>
+    <t>Time Window: 5</t>
+  </si>
+  <si>
+    <t>Time Window for Algorithm: 3</t>
+  </si>
+  <si>
+    <t>NORMAL VERSION</t>
+  </si>
+  <si>
+    <t>OPTIMISED VERSION USING MSE</t>
+  </si>
+  <si>
+    <t>Test Point: 0     Number of Estimated Locations: 10     Mean Distance Error: 4.501510619065057</t>
+  </si>
+  <si>
+    <t>Test Point: 1     Number of Estimated Locations: 7     Mean Distance Error: 4.8088094011944476</t>
+  </si>
+  <si>
+    <t>Test Point: 2     Number of Estimated Locations: 8     Mean Distance Error: 4.358427286799777</t>
+  </si>
+  <si>
+    <t>Test Point: 3     Number of Estimated Locations: 5     Mean Distance Error: 3.5201902505897475</t>
+  </si>
+  <si>
+    <t>Test Point: 4     Number of Estimated Locations: 6     Mean Distance Error: 2.624842781850515</t>
+  </si>
+  <si>
+    <t>Test Point: 5     Number of Estimated Locations: 6     Mean Distance Error: 8.447451004891589</t>
+  </si>
+  <si>
+    <t>Test Point: 6     Number of Estimated Locations: 7     Mean Distance Error: 6.504713875334309</t>
+  </si>
+  <si>
+    <t>Test Point: 7     Number of Estimated Locations: 9     Mean Distance Error: 6.818609202942257</t>
+  </si>
+  <si>
+    <t>Test Point: 8     Number of Estimated Locations: 8     Mean Distance Error: 3.925201919243736</t>
+  </si>
+  <si>
+    <t>Test Point: 9     Number of Estimated Locations: 9     Mean Distance Error: 4.799027511055517</t>
+  </si>
+  <si>
+    <t>Test Point: 10     Number of Estimated Locations: 10     Mean Distance Error: 4.582431751259545</t>
+  </si>
+  <si>
+    <t>Test Point: 11     Number of Estimated Locations: 10     Mean Distance Error: 3.325431549752977</t>
+  </si>
+  <si>
+    <t>Test Point: 12     Number of Estimated Locations: 8     Mean Distance Error: 1.7770546355687684</t>
+  </si>
+  <si>
+    <t>Test Point: 13     Number of Estimated Locations: 7     Mean Distance Error: 2.7083371622276915</t>
+  </si>
+  <si>
+    <t>Test Point: 14     Number of Estimated Locations: 5     Mean Distance Error: 10.490995547627298</t>
+  </si>
+  <si>
+    <t>Overall Mean Distance Error: 4.879535633293548</t>
+  </si>
+  <si>
+    <t>Number of estimated location: 128</t>
+  </si>
+  <si>
+    <t>Test Point: 0     Number of Estimated Locations: 10     Mean Distance Error: 4.082847064026494</t>
+  </si>
+  <si>
+    <t>Test Point: 1     Number of Estimated Locations: 7     Mean Distance Error: 4.8088094010008255</t>
+  </si>
+  <si>
+    <t>Test Point: 2     Number of Estimated Locations: 8     Mean Distance Error: 4.358427286748366</t>
+  </si>
+  <si>
+    <t>Test Point: 3     Number of Estimated Locations: 5     Mean Distance Error: 4.169465149028935</t>
+  </si>
+  <si>
+    <t>Test Point: 4     Number of Estimated Locations: 6     Mean Distance Error: 2.516861191839494</t>
+  </si>
+  <si>
+    <t>Test Point: 5     Number of Estimated Locations: 5     Mean Distance Error: 8.43025189498051</t>
+  </si>
+  <si>
+    <t>Test Point: 6     Number of Estimated Locations: 7     Mean Distance Error: 6.504713875340726</t>
+  </si>
+  <si>
+    <t>Test Point: 7     Number of Estimated Locations: 9     Mean Distance Error: 6.83275175242578</t>
+  </si>
+  <si>
+    <t>Test Point: 8     Number of Estimated Locations: 8     Mean Distance Error: 3.870920357615758</t>
+  </si>
+  <si>
+    <t>Test Point: 9     Number of Estimated Locations: 9     Mean Distance Error: 4.816533739786261</t>
+  </si>
+  <si>
+    <t>Test Point: 10     Number of Estimated Locations: 10     Mean Distance Error: 4.46150435073366</t>
+  </si>
+  <si>
+    <t>Test Point: 11     Number of Estimated Locations: 10     Mean Distance Error: 3.299956542963246</t>
+  </si>
+  <si>
+    <t>Test Point: 12     Number of Estimated Locations: 8     Mean Distance Error: 1.7770546354878394</t>
+  </si>
+  <si>
+    <t>Test Point: 13     Number of Estimated Locations: 7     Mean Distance Error: 2.7083371618443555</t>
+  </si>
+  <si>
+    <t>Test Point: 14     Number of Estimated Locations: 5     Mean Distance Error: 10.490995547707923</t>
+  </si>
+  <si>
+    <t>Overall Mean Distance Error: 4.875295330102011</t>
+  </si>
+  <si>
+    <t>Points Weight 1:3</t>
+  </si>
+  <si>
+    <t>Points Weight 1:0</t>
+  </si>
+  <si>
+    <t>Test Point: 0     Number of Estimated Locations: 10     Mean Distance Error: 4.332825222553025</t>
+  </si>
+  <si>
+    <t>Test Point: 1     Number of Estimated Locations: 7     Mean Distance Error: 4.808809400913537</t>
+  </si>
+  <si>
+    <t>Test Point: 3     Number of Estimated Locations: 5     Mean Distance Error: 3.7818409652981826</t>
+  </si>
+  <si>
+    <t>Test Point: 4     Number of Estimated Locations: 6     Mean Distance Error: 2.513320512310115</t>
+  </si>
+  <si>
+    <t>Test Point: 5     Number of Estimated Locations: 5     Mean Distance Error: 8.001082132934362</t>
+  </si>
+  <si>
+    <t>Test Point: 7     Number of Estimated Locations: 9     Mean Distance Error: 6.823565041039527</t>
+  </si>
+  <si>
+    <t>Test Point: 8     Number of Estimated Locations: 8     Mean Distance Error: 3.8940658591477844</t>
+  </si>
+  <si>
+    <t>Test Point: 9     Number of Estimated Locations: 9     Mean Distance Error: 4.808363666734567</t>
+  </si>
+  <si>
+    <t>Test Point: 10     Number of Estimated Locations: 10     Mean Distance Error: 4.520582066011215</t>
+  </si>
+  <si>
+    <t>Test Point: 11     Number of Estimated Locations: 10     Mean Distance Error: 3.2999565427684696</t>
+  </si>
+  <si>
+    <t>Test Point: 12     Number of Estimated Locations: 8     Mean Distance Error: 1.7770546355441574</t>
+  </si>
+  <si>
+    <t>Test Point: 13     Number of Estimated Locations: 7     Mean Distance Error: 2.7083371619595593</t>
+  </si>
+  <si>
+    <t>Test Point: 14     Number of Estimated Locations: 5     Mean Distance Error: 10.447883520793804</t>
+  </si>
+  <si>
+    <t>Overall Mean Distance Error: 4.838721859339827</t>
+  </si>
+  <si>
+    <t>TESTING WITH POINTS WEIGHT</t>
+  </si>
+  <si>
+    <t>Points Weight 1:1</t>
+  </si>
+  <si>
+    <t>Test Point: 0     Number of Estimated Locations: 10     Mean Distance Error: 4.440825154312095</t>
+  </si>
+  <si>
+    <t>Test Point: 1     Number of Estimated Locations: 7     Mean Distance Error: 4.808809400996389</t>
+  </si>
+  <si>
+    <t>Test Point: 2     Number of Estimated Locations: 8     Mean Distance Error: 4.358427286878782</t>
+  </si>
+  <si>
+    <t>Test Point: 3     Number of Estimated Locations: 5     Mean Distance Error: 3.6108425299356885</t>
+  </si>
+  <si>
+    <t>Test Point: 4     Number of Estimated Locations: 6     Mean Distance Error: 2.573758441793832</t>
+  </si>
+  <si>
+    <t>Test Point: 5     Number of Estimated Locations: 5     Mean Distance Error: 7.892873585701576</t>
+  </si>
+  <si>
+    <t>Test Point: 7     Number of Estimated Locations: 9     Mean Distance Error: 6.819839003796592</t>
+  </si>
+  <si>
+    <t>Test Point: 8     Number of Estimated Locations: 8     Mean Distance Error: 3.9116546435169557</t>
+  </si>
+  <si>
+    <t>Test Point: 9     Number of Estimated Locations: 9     Mean Distance Error: 4.802917428591574</t>
+  </si>
+  <si>
+    <t>Test Point: 10     Number of Estimated Locations: 10     Mean Distance Error: 4.556679289251398</t>
+  </si>
+  <si>
+    <t>Test Point: 11     Number of Estimated Locations: 10     Mean Distance Error: 3.2999565431231517</t>
+  </si>
+  <si>
+    <t>Test Point: 12     Number of Estimated Locations: 8     Mean Distance Error: 1.7770546356039816</t>
+  </si>
+  <si>
+    <t>Test Point: 13     Number of Estimated Locations: 7     Mean Distance Error: 2.708337161859578</t>
+  </si>
+  <si>
+    <t>Test Point: 14     Number of Estimated Locations: 5     Mean Distance Error: 10.414774297773961</t>
+  </si>
+  <si>
+    <t>Overall Mean Distance Error: 4.8320975518979905</t>
+  </si>
+  <si>
+    <t>Points Weight 1:2</t>
+  </si>
+  <si>
+    <t>Test Point: 0     Number of Estimated Locations: 10     Mean Distance Error: 4.5160135111127255</t>
+  </si>
+  <si>
+    <t>Test Point: 1     Number of Estimated Locations: 7     Mean Distance Error: 4.808809401577419</t>
+  </si>
+  <si>
+    <t>Test Point: 2     Number of Estimated Locations: 8     Mean Distance Error: 4.358427286852275</t>
+  </si>
+  <si>
+    <t>Test Point: 3     Number of Estimated Locations: 5     Mean Distance Error: 3.5201902505858667</t>
+  </si>
+  <si>
+    <t>Test Point: 4     Number of Estimated Locations: 6     Mean Distance Error: 2.6248427813522155</t>
+  </si>
+  <si>
+    <t>Test Point: 5     Number of Estimated Locations: 6     Mean Distance Error: 8.447451004805254</t>
+  </si>
+  <si>
+    <t>Test Point: 7     Number of Estimated Locations: 9     Mean Distance Error: 6.818609202790001</t>
+  </si>
+  <si>
+    <t>Test Point: 8     Number of Estimated Locations: 8     Mean Distance Error: 3.9252019190201626</t>
+  </si>
+  <si>
+    <t>Test Point: 9     Number of Estimated Locations: 9     Mean Distance Error: 4.7990275108989335</t>
+  </si>
+  <si>
+    <t>Test Point: 10     Number of Estimated Locations: 10     Mean Distance Error: 4.582431751122656</t>
+  </si>
+  <si>
+    <t>Test Point: 11     Number of Estimated Locations: 10     Mean Distance Error: 3.325431549873876</t>
+  </si>
+  <si>
+    <t>Test Point: 12     Number of Estimated Locations: 8     Mean Distance Error: 1.7770546356107368</t>
+  </si>
+  <si>
+    <t>Test Point: 13     Number of Estimated Locations: 7     Mean Distance Error: 2.7083371622376045</t>
+  </si>
+  <si>
+    <t>Test Point: 14     Number of Estimated Locations: 5     Mean Distance Error: 10.49099554766579</t>
+  </si>
+  <si>
+    <t>Overall Mean Distance Error: 4.8805024927226555</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -55,13 +367,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -73,16 +397,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -361,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:O83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="F82" sqref="F82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -561,9 +888,542 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E17" s="1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" t="s">
+        <v>62</v>
+      </c>
+      <c r="G20" t="s">
+        <v>25</v>
+      </c>
+      <c r="K20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="G21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>15</v>
+      </c>
+      <c r="G30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="G31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>17</v>
+      </c>
+      <c r="G32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>18</v>
+      </c>
+      <c r="G33" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>19</v>
+      </c>
+      <c r="G34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>20</v>
+      </c>
+      <c r="G35" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>21</v>
+      </c>
+      <c r="G36" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>22</v>
+      </c>
+      <c r="G37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>23</v>
+      </c>
+      <c r="G38" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>24</v>
+      </c>
+      <c r="G39" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="2"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>25</v>
+      </c>
+      <c r="D42" t="s">
+        <v>63</v>
+      </c>
+      <c r="G42" t="s">
+        <v>25</v>
+      </c>
+      <c r="K42" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>26</v>
+      </c>
+      <c r="G43" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>45</v>
+      </c>
+      <c r="G44" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="G45" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>46</v>
+      </c>
+      <c r="G46" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>47</v>
+      </c>
+      <c r="G47" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>48</v>
+      </c>
+      <c r="G48" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>49</v>
+      </c>
+      <c r="G49" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>50</v>
+      </c>
+      <c r="G50" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>51</v>
+      </c>
+      <c r="G51" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>52</v>
+      </c>
+      <c r="G52" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>53</v>
+      </c>
+      <c r="G53" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>54</v>
+      </c>
+      <c r="G54" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>55</v>
+      </c>
+      <c r="G55" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>56</v>
+      </c>
+      <c r="G56" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>57</v>
+      </c>
+      <c r="G57" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>58</v>
+      </c>
+      <c r="G58" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>59</v>
+      </c>
+      <c r="G59" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>60</v>
+      </c>
+      <c r="G60" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>61</v>
+      </c>
+      <c r="G61" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>25</v>
+      </c>
+      <c r="D64" t="s">
+        <v>95</v>
+      </c>
+      <c r="G64" t="s">
+        <v>25</v>
+      </c>
+      <c r="K64" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>26</v>
+      </c>
+      <c r="G65" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>45</v>
+      </c>
+      <c r="G66" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>8</v>
+      </c>
+      <c r="G67" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>80</v>
+      </c>
+      <c r="G68" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>81</v>
+      </c>
+      <c r="G69" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>82</v>
+      </c>
+      <c r="G70" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>83</v>
+      </c>
+      <c r="G71" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>84</v>
+      </c>
+      <c r="G72" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>85</v>
+      </c>
+      <c r="G73" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>35</v>
+      </c>
+      <c r="G74" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>86</v>
+      </c>
+      <c r="G75" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>87</v>
+      </c>
+      <c r="G76" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>88</v>
+      </c>
+      <c r="G77" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>89</v>
+      </c>
+      <c r="G78" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>90</v>
+      </c>
+      <c r="G79" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>91</v>
+      </c>
+      <c r="G80" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>92</v>
+      </c>
+      <c r="G81" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>93</v>
+      </c>
+      <c r="G82" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>94</v>
+      </c>
+      <c r="G83" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>